<commit_message>
update camera intrinsic calibration
</commit_message>
<xml_diff>
--- a/camera_intrinsic/data/20221221_zhoushan/IRayCamera.xlsx
+++ b/camera_intrinsic/data/20221221_zhoushan/IRayCamera.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sensors_calibration_v2.1\camera_intrinsic\data\20221221_zhoushan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95F3554-E60C-4378-9F6A-B04207D48AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2EB0B-4F13-4A92-A8F5-38970B9605C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28656" yWindow="2268" windowWidth="27648" windowHeight="14592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>